<commit_message>
Added a few extra calculations to uck design summary xls's for annual review
</commit_message>
<xml_diff>
--- a/uck2_collaboration/simulation_results/designing_enzyme/design_round_2/0_Models summary.xlsx
+++ b/uck2_collaboration/simulation_results/designing_enzyme/design_round_2/0_Models summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhlub\Documents\khare_lab\uck2_collaboration\designing_enzyme\design_round_2\representative_designs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhlub\Documents\khare_lab\uck2_collaboration\simulation_results\designing_enzyme\design_round_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4603C8A9-4194-4B9D-B148-0BFEC24E0218}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E505C50-8DBD-44BB-A576-9020EDD42030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26850" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{D28C5CCA-792B-47FE-BA29-6CC0D4CE0B61}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{D28C5CCA-792B-47FE-BA29-6CC0D4CE0B61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="69">
   <si>
     <t>pdb_name</t>
   </si>
@@ -169,6 +169,75 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>Substrate</t>
+  </si>
+  <si>
+    <t>F/H</t>
+  </si>
+  <si>
+    <t>A/S</t>
+  </si>
+  <si>
+    <t>I/W</t>
+  </si>
+  <si>
+    <t>A/G</t>
+  </si>
+  <si>
+    <t>F/N</t>
+  </si>
+  <si>
+    <t>N/Y</t>
+  </si>
+  <si>
+    <t>T/V/W</t>
+  </si>
+  <si>
+    <t>F/Y</t>
+  </si>
+  <si>
+    <t>A/G/H</t>
+  </si>
+  <si>
+    <t>5AM</t>
+  </si>
+  <si>
+    <t>5CP</t>
+  </si>
+  <si>
+    <t>5DZ</t>
+  </si>
+  <si>
+    <t>C35AM</t>
+  </si>
+  <si>
+    <t>F/L/Y</t>
+  </si>
+  <si>
+    <t>F/G/H</t>
+  </si>
+  <si>
+    <t>T/W</t>
+  </si>
+  <si>
+    <t>Cyclo</t>
+  </si>
+  <si>
+    <t>A/L</t>
+  </si>
+  <si>
+    <t>A/L/Y</t>
+  </si>
+  <si>
+    <t>A/F/G</t>
+  </si>
+  <si>
+    <t>A/Y</t>
+  </si>
+  <si>
+    <t>M5</t>
   </si>
 </sst>
 </file>
@@ -527,20 +596,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C4773A-974C-4116-A018-A79A2585B991}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -1247,6 +1318,146 @@
         <v>18</v>
       </c>
     </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" t="s">
+        <v>52</v>
+      </c>
+      <c r="H22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I2:O18">
     <sortCondition ref="O2:O18"/>

</xml_diff>